<commit_message>
Initial protobuf take with a functional Java implementation
</commit_message>
<xml_diff>
--- a/data/BioGears.xlsx
+++ b/data/BioGears.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\BioGears\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\BioGears\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="555" windowWidth="15090" windowHeight="7350" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="6" r:id="rId1"/>
@@ -17,16 +17,17 @@
     <sheet name="Compounds" sheetId="8" r:id="rId3"/>
     <sheet name="Environment" sheetId="9" r:id="rId4"/>
     <sheet name="Nutrition" sheetId="10" r:id="rId5"/>
-    <sheet name="Stabilization" sheetId="11" r:id="rId6"/>
-    <sheet name="Configuration" sheetId="12" r:id="rId7"/>
-    <sheet name="Tissue" sheetId="13" r:id="rId8"/>
+    <sheet name="ECG" sheetId="14" r:id="rId6"/>
+    <sheet name="Stabilization" sheetId="11" r:id="rId7"/>
+    <sheet name="Configuration" sheetId="12" r:id="rId8"/>
+    <sheet name="Tissue" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4479" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4489" uniqueCount="692">
   <si>
     <t>Name</t>
   </si>
@@ -2080,6 +2081,39 @@
   </si>
   <si>
     <t>168.038 g/mol</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Rhythm</t>
+  </si>
+  <si>
+    <t>ElectricPotential</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>NormalSinus</t>
+  </si>
+  <si>
+    <t>-0.039,-0.032,-0.026,-0.021,-0.01,-0.001,0,0.006,0.009,-0.002,-0.004,0.006,0.006,0.01,0.022,0.043,0.052,0.054,0.062,0.071,0.068,0.061,0.057,0.061,0.06,0.046,0.042,0.035,0.017,0.004,-0.001,-0.009,-0.01,-0.012,-0.024,-0.031,-0.038,-0.048,-0.049,-0.051,-0.049,-0.048,-0.057,-0.062,-0.06,-0.059,-0.06,-0.065,-0.067,-0.067,-0.076,-0.089,-0.085,-0.074,-0.072,-0.073,-0.074,-0.077,-0.078,-0.079,-0.083,-0.084,-0.074,-0.078,-0.09,-0.083,-0.083,-0.084,-0.074,-0.073,-0.076,-0.077,-0.078,-0.065,-0.04,-0.01,0.033,0.081,0.12,0.157,0.193,0.243,0.319,0.396,0.461,0.513,0.568,0.629,0.658,0.668,0.623,0.453,0.232,0.106,0.063,0.017,-0.006,-0.011,-0.042,-0.077,-0.089,-0.087,-0.077,-0.066,-0.059,-0.052,-0.044,-0.039,-0.043,-0.038,-0.028,-0.028,-0.032,-0.032,-0.033,-0.035,-0.038,-0.042,-0.04,-0.035,-0.029,-0.031,-0.038,-0.035,-0.032,-0.037,-0.037,-0.034,-0.033,-0.033,-0.035,-0.029,-0.026,-0.029,-0.026,-0.023,-0.024,-0.021,-0.022,-0.018,-0.015,-0.016,-0.018,-0.024,-0.023,-0.021,-0.02,-0.011,-0.007,-0.007,-0.006,-0.002,0.002,0.001,0.002,0.006,0.004,0.001,0.007,0.013,0.017,0.018,0.022,0.022,0.02,0.023,0.022,0.021,0.031,0.034,0.033,0.037,0.04,0.045,0.044,0.042,0.049,0.055,0.06,0.066,0.068,0.071,0.073,0.074,0.083,0.087,0.085,0.093,0.093,0.098,0.114,0.115,0.117,0.125,0.126,0.128,0.133,0.142,0.145,0.145,0.153,0.161,0.161,0.161,0.17,0.173,0.176,0.181,0.183,0.19,0.194,0.195,0.2,0.203,0.205,0.204,0.206,0.206,0.201,0.204,0.209,0.21,0.214,0.212,0.2,0.2,0.205,0.206,0.209,0.204,0.198,0.193,0.178,0.17,0.167,0.162,0.157,0.147,0.139,0.131,0.111,0.1,0.093,0.081,0.077,0.071,0.062,0.061,0.05,0.039,0.032,0.018,0.012,0.007,-0.005,-0.007,-0.006,-0.013,-0.018,-0.02,-0.026,-0.028,-0.027,-0.034,-0.038,-0.039,-0.035,-0.033,-0.037,-0.042,-0.045,-0.045,-0.04,-0.043,-0.046,-0.037,-0.035,-0.039,-0.035,-0.037,-0.037,-0.035,-0.039 mV</t>
+  </si>
+  <si>
+    <t>0,0.002,0.004,0.006,0.008,0.01,0.012,0.014,0.016,0.018,0.02,0.022,0.024,0.026,0.028,0.03,0.032,0.034,0.036,0.038,0.04,0.043,0.045,0.047,0.049,0.051,0.053,0.055,0.057,0.059,0.061,0.063,0.065,0.067,0.069,0.071,0.073,0.075,0.077,0.079,0.081,0.083,0.085,0.087,0.089,0.091,0.093,0.095,0.097,0.099,0.101,0.103,0.105,0.107,0.109,0.111,0.113,0.115,0.117,0.119,0.121,0.123,0.125,0.127,0.129,0.131,0.133,0.135,0.137,0.139,0.141,0.143,0.145,0.147,0.149,0.151,0.153,0.155,0.157,0.159,0.161,0.163,0.165,0.168,0.17,0.172,0.174,0.176,0.178,0.18,0.182,0.184,0.186,0.188,0.19,0.192,0.194,0.196,0.198,0.2,0.202,0.204,0.206,0.208,0.21,0.212,0.214,0.216,0.218,0.22,0.222,0.224,0.226,0.228,0.23,0.232,0.234,0.236,0.238,0.24,0.242,0.244,0.246,0.248,0.25,0.252,0.254,0.256,0.258,0.26,0.262,0.264,0.266,0.268,0.27,0.272,0.274,0.276,0.278,0.28,0.282,0.284,0.286,0.288,0.29,0.293,0.295,0.297,0.299,0.301,0.303,0.305,0.307,0.309,0.311,0.313,0.315,0.317,0.319,0.321,0.323,0.325,0.327,0.329,0.331,0.333,0.335,0.337,0.339,0.341,0.343,0.345,0.347,0.349,0.351,0.353,0.355,0.357,0.359,0.361,0.363,0.365,0.367,0.369,0.371,0.373,0.375,0.377,0.379,0.381,0.383,0.385,0.387,0.389,0.391,0.393,0.395,0.397,0.399,0.401,0.403,0.405,0.407,0.409,0.411,0.413,0.415,0.418,0.42,0.422,0.424,0.426,0.428,0.43,0.432,0.434,0.436,0.438,0.44,0.442,0.444,0.446,0.448,0.45,0.452,0.454,0.456,0.458,0.46,0.462,0.464,0.466,0.468,0.47,0.472,0.474,0.476,0.478,0.48,0.482,0.484,0.486,0.488,0.49,0.492,0.494,0.496,0.498,0.5,0.502,0.504,0.506,0.508,0.51,0.512,0.514,0.516,0.518,0.52,0.522,0.524,0.526,0.528,0.53,0.532,0.534,0.536,0.538,0.54,0.543,0.545,0.547,0.549,0.551,0.553,0.555,0.557,0.559,0.561,0.563,0.565,0.567,0.569 s</t>
+  </si>
+  <si>
+    <t>ECG consists of a Lead 3 Normal Sinus waveform retrieved from Physionet @cite goldberger2000physiobank.
+ Specifically, the waveform used is from the Stress Recognition in Automobile Drivers study done by Healey and Picard, file
+ drive04.dat, the ECG output from time 1:58.772 - 1:59.349 @cite healey2005detecting. This data was chosen because of its clear
+ display of all features seen in a Normal Sinus rhythm.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>StandardECG</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -2610,6 +2644,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2619,7 +2744,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3055,6 +3180,66 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -4468,9 +4653,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FC74"/>
+  <dimension ref="A1:EX74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -24319,10 +24504,145 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="45" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="196" t="s">
+        <v>690</v>
+      </c>
+      <c r="B2" s="195" t="s">
+        <v>689</v>
+      </c>
+      <c r="C2" s="192"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
+      <c r="M2" s="193"/>
+      <c r="N2" s="193"/>
+      <c r="O2" s="194"/>
+    </row>
+    <row r="3" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>682</v>
+      </c>
+      <c r="B3" s="54">
+        <v>3</v>
+      </c>
+      <c r="C3" s="186"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="187"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="187"/>
+      <c r="L3" s="187"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
+      <c r="O3" s="188"/>
+    </row>
+    <row r="4" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>683</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>686</v>
+      </c>
+      <c r="C4" s="189"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+      <c r="L4" s="190"/>
+      <c r="M4" s="190"/>
+      <c r="N4" s="190"/>
+      <c r="O4" s="191"/>
+    </row>
+    <row r="5" spans="1:15" s="37" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="177" t="s">
+        <v>684</v>
+      </c>
+      <c r="B5" s="178" t="s">
+        <v>687</v>
+      </c>
+      <c r="C5" s="180"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="181"/>
+      <c r="G5" s="181"/>
+      <c r="H5" s="181"/>
+      <c r="I5" s="181"/>
+      <c r="J5" s="181"/>
+      <c r="K5" s="181"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="181"/>
+      <c r="N5" s="181"/>
+      <c r="O5" s="182"/>
+    </row>
+    <row r="6" spans="1:15" s="177" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A6" s="177" t="s">
+        <v>685</v>
+      </c>
+      <c r="B6" s="179" t="s">
+        <v>688</v>
+      </c>
+      <c r="C6" s="183"/>
+      <c r="D6" s="184"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="184"/>
+      <c r="H6" s="184"/>
+      <c r="I6" s="184"/>
+      <c r="J6" s="184"/>
+      <c r="K6" s="184"/>
+      <c r="L6" s="184"/>
+      <c r="M6" s="184"/>
+      <c r="N6" s="184"/>
+      <c r="O6" s="185"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C5:O6"/>
+    <mergeCell ref="C3:O4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26756,7 +27076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C58"/>
   <sheetViews>
@@ -27218,7 +27538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N105"/>
   <sheetViews>

</xml_diff>